<commit_message>
General functionality moved to core.clj.  Loading all sheets in SupplyDemand workbook once as records now.
</commit_message>
<xml_diff>
--- a/resources/SupplyDemand_input.xlsx
+++ b/resources/SupplyDemand_input.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="supplydemand" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="SupplyDemand" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1974,10 +1974,10 @@
   <dimension ref="A1:T300"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.27"/>
@@ -1988,14 +1988,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="8.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="11.16"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Saving the forge xlsx worksheet as tab delimited now, had to pull in the docjure dependency for now.
</commit_message>
<xml_diff>
--- a/resources/SupplyDemand_input.xlsx
+++ b/resources/SupplyDemand_input.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="SupplyDemand" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="SRC_By_Day" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="644">
   <si>
     <t xml:space="preserve">SRC2</t>
   </si>
@@ -1874,6 +1875,96 @@
   </si>
   <si>
     <t xml:space="preserve">CONTRACTING SPT BDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FwdStation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH IIa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH IIb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branc Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch Label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 0001
+TP 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 0009
+TP 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 0017
+TP 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 0025
+TP 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 0033
+TP 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 0041
+TP 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 0049
+TP 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 0057
+TP 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 0065
+TP 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 0073
+TP 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 0081
+TP 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 0089
+TP 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ponies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Army</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buffalos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Army Strength</t>
   </si>
 </sst>
 </file>
@@ -1883,7 +1974,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1905,6 +1996,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1949,9 +2046,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -20602,4 +20703,260 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:R6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="7" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.93"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="0" t="s">
+        <v>618</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>619</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>620</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>622</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>623</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>624</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>625</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>626</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>639</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>381</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>640</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>641</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>642</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>590</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>640</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>641</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>643</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>362377</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Now replacing idaho and cannibal demands and supply in the base marathon workbook.
</commit_message>
<xml_diff>
--- a/resources/SupplyDemand_input.xlsx
+++ b/resources/SupplyDemand_input.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SupplyDemand" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="SRC_By_Day" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="policy_map" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="646">
   <si>
     <t xml:space="preserve">SRC2</t>
   </si>
@@ -1965,6 +1966,12 @@
   </si>
   <si>
     <t xml:space="preserve">Total Army Strength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CompositePolicyName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAA_2125_R2_RC</t>
   </si>
 </sst>
 </file>
@@ -1974,7 +1981,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2002,6 +2009,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2046,13 +2059,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2074,11 +2091,11 @@
   </sheetPr>
   <dimension ref="A1:T300"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.27"/>
@@ -2089,14 +2106,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="8.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="11.16"/>
   </cols>
   <sheetData>
@@ -20716,17 +20733,17 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="7" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.93"/>
   </cols>
   <sheetData>
@@ -20948,6 +20965,49 @@
       </c>
       <c r="R6" s="0" t="n">
         <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.33"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>645</v>
       </c>
     </row>
   </sheetData>

</xml_diff>